<commit_message>
this is my second visual
</commit_message>
<xml_diff>
--- a/Covid-19 dataset.xlsx
+++ b/Covid-19 dataset.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FJWU\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FJWU\Desktop\DS-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3567BBD-D2A0-4D14-B8C9-D5E550EB415F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4EF115-F54A-4FCC-8B95-332315450474}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="425">
   <si>
     <t>Cumulative</t>
   </si>
@@ -887,9 +887,6 @@
   </si>
   <si>
     <t>Training and orientation sessions for the health staff at Hyderabad started.   •</t>
-  </si>
-  <si>
-    <t>KP &amp; TD</t>
   </si>
   <si>
     <t>24 High Dependency Units established across KP.  •</t>
@@ -1860,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K454"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="D266" workbookViewId="0">
+      <selection activeCell="A469" sqref="A469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17784,25 +17781,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>424</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>425</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -18175,7 +18172,7 @@
   <dimension ref="A1:BA239"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60609,9 +60606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{139A6597-8FAB-4193-A383-F9E7C236E520}">
   <dimension ref="A1:D167"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -60693,44 +60688,44 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
         <v>247</v>
-      </c>
-      <c r="B6" t="s">
-        <v>248</v>
       </c>
       <c r="C6" s="3">
         <v>43901</v>
       </c>
       <c r="D6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C7" s="3">
         <v>43901</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C8" s="3">
         <v>43901</v>
       </c>
       <c r="D8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -60738,13 +60733,13 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C9" s="3">
         <v>43901</v>
       </c>
       <c r="D9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -60752,13 +60747,13 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="3">
         <v>43902</v>
       </c>
       <c r="D10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -60766,13 +60761,13 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C11" s="3">
         <v>43902</v>
       </c>
       <c r="D11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -60780,13 +60775,13 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C12" s="3">
         <v>43902</v>
       </c>
       <c r="D12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -60794,41 +60789,41 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C13" s="3">
         <v>43902</v>
       </c>
       <c r="D13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C14" s="3">
         <v>43902</v>
       </c>
       <c r="D14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C15" s="3">
         <v>43902</v>
       </c>
       <c r="D15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -60836,13 +60831,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C16" s="3">
         <v>43902</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -60850,13 +60845,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C17" s="3">
         <v>43902</v>
       </c>
       <c r="D17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -60864,13 +60859,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C18" s="3">
         <v>43903</v>
       </c>
       <c r="D18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -60878,13 +60873,13 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C19" s="3">
         <v>43903</v>
       </c>
       <c r="D19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -60892,13 +60887,13 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20" s="3">
         <v>43903</v>
       </c>
       <c r="D20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -60906,41 +60901,41 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C21" s="3">
         <v>43903</v>
       </c>
       <c r="D21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C22" s="3">
         <v>43903</v>
       </c>
       <c r="D22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C23" s="3">
         <v>43903</v>
       </c>
       <c r="D23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -60948,13 +60943,13 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C24" s="3">
         <v>43903</v>
       </c>
       <c r="D24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -60962,13 +60957,13 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C25" s="3">
         <v>43903</v>
       </c>
       <c r="D25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -60976,13 +60971,13 @@
         <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C26" s="3">
         <v>43903</v>
       </c>
       <c r="D26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -60990,13 +60985,13 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="3">
         <v>43904</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -61004,13 +60999,13 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C28" s="3">
         <v>43904</v>
       </c>
       <c r="D28" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -61018,27 +61013,27 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C29" s="3">
         <v>43904</v>
       </c>
       <c r="D29" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C30" s="3">
         <v>43904</v>
       </c>
       <c r="D30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -61046,13 +61041,13 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C31" s="3">
         <v>43904</v>
       </c>
       <c r="D31" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -61060,13 +61055,13 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C32" s="3">
         <v>43904</v>
       </c>
       <c r="D32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -61074,13 +61069,13 @@
         <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C33" s="3">
         <v>43904</v>
       </c>
       <c r="D33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -61088,13 +61083,13 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C34" s="3">
         <v>43905</v>
       </c>
       <c r="D34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -61102,13 +61097,13 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C35" s="3">
         <v>43905</v>
       </c>
       <c r="D35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -61116,13 +61111,13 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C36" s="3">
         <v>43905</v>
       </c>
       <c r="D36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -61130,13 +61125,13 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C37" s="3">
         <v>43905</v>
       </c>
       <c r="D37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -61144,13 +61139,13 @@
         <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C38" s="3">
         <v>43905</v>
       </c>
       <c r="D38" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -61158,27 +61153,27 @@
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C39" s="3">
         <v>43905</v>
       </c>
       <c r="D39" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C40" s="3">
         <v>43905</v>
       </c>
       <c r="D40" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -61186,13 +61181,13 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C41" s="3">
         <v>43905</v>
       </c>
       <c r="D41" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -61200,13 +61195,13 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C42" s="3">
         <v>43905</v>
       </c>
       <c r="D42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -61214,13 +61209,13 @@
         <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C43" s="3">
         <v>43905</v>
       </c>
       <c r="D43" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -61228,13 +61223,13 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C44" s="3">
         <v>43906</v>
       </c>
       <c r="D44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -61242,13 +61237,13 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C45" s="3">
         <v>43906</v>
       </c>
       <c r="D45" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -61256,13 +61251,13 @@
         <v>13</v>
       </c>
       <c r="B46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C46" s="3">
         <v>43906</v>
       </c>
       <c r="D46" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -61270,27 +61265,27 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C47" s="3">
         <v>43906</v>
       </c>
       <c r="D47" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C48" s="3">
         <v>43906</v>
       </c>
       <c r="D48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -61298,13 +61293,13 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C49" s="3">
         <v>43906</v>
       </c>
       <c r="D49" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -61312,13 +61307,13 @@
         <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C50" s="3">
         <v>43906</v>
       </c>
       <c r="D50" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -61326,13 +61321,13 @@
         <v>18</v>
       </c>
       <c r="B51" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C51" s="3">
         <v>43906</v>
       </c>
       <c r="D51" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -61340,13 +61335,13 @@
         <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C52" s="3">
         <v>43907</v>
       </c>
       <c r="D52" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -61354,13 +61349,13 @@
         <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C53" s="3">
         <v>43907</v>
       </c>
       <c r="D53" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -61368,13 +61363,13 @@
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C54" s="3">
         <v>43907</v>
       </c>
       <c r="D54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -61382,13 +61377,13 @@
         <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C55" s="3">
         <v>43907</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -61396,27 +61391,27 @@
         <v>12</v>
       </c>
       <c r="B56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C56" s="3">
         <v>43907</v>
       </c>
       <c r="D56" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C57" s="3">
         <v>43907</v>
       </c>
       <c r="D57" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -61424,13 +61419,13 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C58" s="3">
         <v>43907</v>
       </c>
       <c r="D58" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -61438,13 +61433,13 @@
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C59" s="3">
         <v>43907</v>
       </c>
       <c r="D59" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -61452,13 +61447,13 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C60" s="3">
         <v>43908</v>
       </c>
       <c r="D60" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -61466,13 +61461,13 @@
         <v>13</v>
       </c>
       <c r="B61" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C61" s="3">
         <v>43908</v>
       </c>
       <c r="D61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -61480,13 +61475,13 @@
         <v>13</v>
       </c>
       <c r="B62" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C62" s="3">
         <v>43908</v>
       </c>
       <c r="D62" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -61494,27 +61489,27 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C63" s="3">
         <v>43908</v>
       </c>
       <c r="D63" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C64" s="3">
         <v>43908</v>
       </c>
       <c r="D64" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -61522,13 +61517,13 @@
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C65" s="3">
         <v>43908</v>
       </c>
       <c r="D65" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -61536,13 +61531,13 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C66" s="3">
         <v>43908</v>
       </c>
       <c r="D66" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -61550,13 +61545,13 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C67" s="3">
         <v>43908</v>
       </c>
       <c r="D67" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -61564,13 +61559,13 @@
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C68" s="3">
         <v>43909</v>
       </c>
       <c r="D68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -61578,13 +61573,13 @@
         <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C69" s="3">
         <v>43909</v>
       </c>
       <c r="D69" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -61592,27 +61587,27 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C70" s="3">
         <v>43909</v>
       </c>
       <c r="D70" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C71" s="3">
         <v>43909</v>
       </c>
       <c r="D71" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -61620,13 +61615,13 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C72" s="3">
         <v>43909</v>
       </c>
       <c r="D72" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -61634,13 +61629,13 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C73" s="3">
         <v>43909</v>
       </c>
       <c r="D73" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -61648,13 +61643,13 @@
         <v>16</v>
       </c>
       <c r="B74" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C74" s="3">
         <v>43910</v>
       </c>
       <c r="D74" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -61662,13 +61657,13 @@
         <v>16</v>
       </c>
       <c r="B75" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C75" s="3">
         <v>43910</v>
       </c>
       <c r="D75" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -61676,13 +61671,13 @@
         <v>13</v>
       </c>
       <c r="B76" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C76" s="3">
         <v>43910</v>
       </c>
       <c r="D76" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -61690,27 +61685,27 @@
         <v>12</v>
       </c>
       <c r="B77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C77" s="3">
         <v>43910</v>
       </c>
       <c r="D77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B78" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C78" s="3">
         <v>43910</v>
       </c>
       <c r="D78" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -61718,13 +61713,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C79" s="3">
         <v>43910</v>
       </c>
       <c r="D79" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -61732,13 +61727,13 @@
         <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C80" s="3">
         <v>43910</v>
       </c>
       <c r="D80" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -61746,13 +61741,13 @@
         <v>16</v>
       </c>
       <c r="B81" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C81" s="3">
         <v>43911</v>
       </c>
       <c r="D81" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -61760,13 +61755,13 @@
         <v>13</v>
       </c>
       <c r="B82" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C82" s="3">
         <v>43911</v>
       </c>
       <c r="D82" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -61774,13 +61769,13 @@
         <v>12</v>
       </c>
       <c r="B83" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C83" s="3">
         <v>43911</v>
       </c>
       <c r="D83" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -61788,27 +61783,27 @@
         <v>12</v>
       </c>
       <c r="B84" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C84" s="3">
         <v>43911</v>
       </c>
       <c r="D84" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B85" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C85" s="3">
         <v>43911</v>
       </c>
       <c r="D85" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -61816,13 +61811,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C86" s="3">
         <v>43911</v>
       </c>
       <c r="D86" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -61830,13 +61825,13 @@
         <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C87" s="3">
         <v>43911</v>
       </c>
       <c r="D87" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -61844,13 +61839,13 @@
         <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C88" s="3">
         <v>43912</v>
       </c>
       <c r="D88" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -61858,13 +61853,13 @@
         <v>16</v>
       </c>
       <c r="B89" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C89" s="3">
         <v>43912</v>
       </c>
       <c r="D89" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -61872,13 +61867,13 @@
         <v>13</v>
       </c>
       <c r="B90" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C90" s="3">
         <v>43912</v>
       </c>
       <c r="D90" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -61886,27 +61881,27 @@
         <v>12</v>
       </c>
       <c r="B91" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C91" s="3">
         <v>43912</v>
       </c>
       <c r="D91" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C92" s="3">
         <v>43912</v>
       </c>
       <c r="D92" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -61914,13 +61909,13 @@
         <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C93" s="3">
         <v>43912</v>
       </c>
       <c r="D93" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -61928,13 +61923,13 @@
         <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C94" s="3">
         <v>43912</v>
       </c>
       <c r="D94" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -61942,13 +61937,13 @@
         <v>16</v>
       </c>
       <c r="B95" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C95" s="3">
         <v>43913</v>
       </c>
       <c r="D95" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -61956,13 +61951,13 @@
         <v>13</v>
       </c>
       <c r="B96" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C96" s="3">
         <v>43913</v>
       </c>
       <c r="D96" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -61970,27 +61965,27 @@
         <v>12</v>
       </c>
       <c r="B97" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C97" s="3">
         <v>43913</v>
       </c>
       <c r="D97" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C98" s="3">
         <v>43913</v>
       </c>
       <c r="D98" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -61998,13 +61993,13 @@
         <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C99" s="3">
         <v>43913</v>
       </c>
       <c r="D99" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -62012,13 +62007,13 @@
         <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C100" s="3">
         <v>43913</v>
       </c>
       <c r="D100" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -62026,13 +62021,13 @@
         <v>16</v>
       </c>
       <c r="B101" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C101" s="3">
         <v>43914</v>
       </c>
       <c r="D101" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -62040,13 +62035,13 @@
         <v>13</v>
       </c>
       <c r="B102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C102" s="3">
         <v>43914</v>
       </c>
       <c r="D102" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -62054,27 +62049,27 @@
         <v>12</v>
       </c>
       <c r="B103" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C103" s="3">
         <v>43914</v>
       </c>
       <c r="D103" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B104" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C104" s="3">
         <v>43914</v>
       </c>
       <c r="D104" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -62082,13 +62077,13 @@
         <v>17</v>
       </c>
       <c r="B105" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C105" s="3">
         <v>43914</v>
       </c>
       <c r="D105" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -62096,13 +62091,13 @@
         <v>18</v>
       </c>
       <c r="B106" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C106" s="3">
         <v>43914</v>
       </c>
       <c r="D106" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -62110,13 +62105,13 @@
         <v>16</v>
       </c>
       <c r="B107" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C107" s="3">
         <v>43915</v>
       </c>
       <c r="D107" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -62124,13 +62119,13 @@
         <v>13</v>
       </c>
       <c r="B108" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C108" s="3">
         <v>43915</v>
       </c>
       <c r="D108" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -62138,27 +62133,27 @@
         <v>12</v>
       </c>
       <c r="B109" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C109" s="3">
         <v>43915</v>
       </c>
       <c r="D109" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B110" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C110" s="3">
         <v>43915</v>
       </c>
       <c r="D110" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -62166,13 +62161,13 @@
         <v>18</v>
       </c>
       <c r="B111" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C111" s="3">
         <v>43915</v>
       </c>
       <c r="D111" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -62180,13 +62175,13 @@
         <v>16</v>
       </c>
       <c r="B112" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C112" s="3">
         <v>43916</v>
       </c>
       <c r="D112" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -62194,13 +62189,13 @@
         <v>13</v>
       </c>
       <c r="B113" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C113" s="3">
         <v>43916</v>
       </c>
       <c r="D113" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -62208,27 +62203,27 @@
         <v>12</v>
       </c>
       <c r="B114" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C114" s="3">
         <v>43916</v>
       </c>
       <c r="D114" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>247</v>
+        <v>15</v>
       </c>
       <c r="B115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C115" s="3">
         <v>43916</v>
       </c>
       <c r="D115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -62236,13 +62231,13 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C116" s="3">
         <v>43916</v>
       </c>
       <c r="D116" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -62250,13 +62245,13 @@
         <v>18</v>
       </c>
       <c r="B117" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C117" s="3">
         <v>43916</v>
       </c>
       <c r="D117" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -62264,13 +62259,13 @@
         <v>16</v>
       </c>
       <c r="B118" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C118" s="3">
         <v>43917</v>
       </c>
       <c r="D118" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -62278,13 +62273,13 @@
         <v>13</v>
       </c>
       <c r="B119" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C119" s="3">
         <v>43917</v>
       </c>
       <c r="D119" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -62292,13 +62287,13 @@
         <v>12</v>
       </c>
       <c r="B120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C120" s="3">
         <v>43917</v>
       </c>
       <c r="D120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -62306,13 +62301,13 @@
         <v>14</v>
       </c>
       <c r="B121" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C121" s="3">
         <v>43917</v>
       </c>
       <c r="D121" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -62320,13 +62315,13 @@
         <v>17</v>
       </c>
       <c r="B122" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C122" s="3">
         <v>43917</v>
       </c>
       <c r="D122" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -62334,13 +62329,13 @@
         <v>18</v>
       </c>
       <c r="B123" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C123" s="3">
         <v>43917</v>
       </c>
       <c r="D123" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -62348,13 +62343,13 @@
         <v>16</v>
       </c>
       <c r="B124" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C124" s="3">
         <v>43918</v>
       </c>
       <c r="D124" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -62362,13 +62357,13 @@
         <v>13</v>
       </c>
       <c r="B125" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C125" s="3">
         <v>43918</v>
       </c>
       <c r="D125" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -62376,13 +62371,13 @@
         <v>12</v>
       </c>
       <c r="B126" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C126" s="3">
         <v>43918</v>
       </c>
       <c r="D126" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -62390,13 +62385,13 @@
         <v>14</v>
       </c>
       <c r="B127" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C127" s="3">
         <v>43918</v>
       </c>
       <c r="D127" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -62404,13 +62399,13 @@
         <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C128" s="3">
         <v>43918</v>
       </c>
       <c r="D128" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -62418,13 +62413,13 @@
         <v>18</v>
       </c>
       <c r="B129" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C129" s="3">
         <v>43918</v>
       </c>
       <c r="D129" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -62432,13 +62427,13 @@
         <v>16</v>
       </c>
       <c r="B130" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C130" s="3">
         <v>43919</v>
       </c>
       <c r="D130" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -62446,13 +62441,13 @@
         <v>13</v>
       </c>
       <c r="B131" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C131" s="3">
         <v>43919</v>
       </c>
       <c r="D131" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -62460,13 +62455,13 @@
         <v>12</v>
       </c>
       <c r="B132" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C132" s="3">
         <v>43919</v>
       </c>
       <c r="D132" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -62474,13 +62469,13 @@
         <v>14</v>
       </c>
       <c r="B133" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C133" s="3">
         <v>43919</v>
       </c>
       <c r="D133" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -62488,13 +62483,13 @@
         <v>17</v>
       </c>
       <c r="B134" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C134" s="3">
         <v>43919</v>
       </c>
       <c r="D134" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -62502,13 +62497,13 @@
         <v>18</v>
       </c>
       <c r="B135" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C135" s="3">
         <v>43919</v>
       </c>
       <c r="D135" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -62516,13 +62511,13 @@
         <v>16</v>
       </c>
       <c r="B136" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C136" s="3">
         <v>43920</v>
       </c>
       <c r="D136" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -62530,13 +62525,13 @@
         <v>13</v>
       </c>
       <c r="B137" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C137" s="3">
         <v>43920</v>
       </c>
       <c r="D137" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -62544,13 +62539,13 @@
         <v>12</v>
       </c>
       <c r="B138" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C138" s="3">
         <v>43920</v>
       </c>
       <c r="D138" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -62558,13 +62553,13 @@
         <v>14</v>
       </c>
       <c r="B139" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C139" s="3">
         <v>43920</v>
       </c>
       <c r="D139" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -62572,13 +62567,13 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C140" s="3">
         <v>43920</v>
       </c>
       <c r="D140" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -62586,13 +62581,13 @@
         <v>18</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C141" s="3">
         <v>43920</v>
       </c>
       <c r="D141" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -62600,13 +62595,13 @@
         <v>16</v>
       </c>
       <c r="B142" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C142" s="3">
         <v>43921</v>
       </c>
       <c r="D142" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -62614,13 +62609,13 @@
         <v>16</v>
       </c>
       <c r="B143" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C143" s="3">
         <v>43921</v>
       </c>
       <c r="D143" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -62628,13 +62623,13 @@
         <v>13</v>
       </c>
       <c r="B144" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C144" s="3">
         <v>43921</v>
       </c>
       <c r="D144" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -62642,13 +62637,13 @@
         <v>12</v>
       </c>
       <c r="B145" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C145" s="3">
         <v>43921</v>
       </c>
       <c r="D145" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -62656,13 +62651,13 @@
         <v>14</v>
       </c>
       <c r="B146" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C146" s="3">
         <v>43921</v>
       </c>
       <c r="D146" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -62670,13 +62665,13 @@
         <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C147" s="3">
         <v>43921</v>
       </c>
       <c r="D147" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -62684,13 +62679,13 @@
         <v>18</v>
       </c>
       <c r="B148" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C148" s="3">
         <v>43921</v>
       </c>
       <c r="D148" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -62698,13 +62693,13 @@
         <v>16</v>
       </c>
       <c r="B149" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C149" s="3">
         <v>43922</v>
       </c>
       <c r="D149" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -62712,13 +62707,13 @@
         <v>13</v>
       </c>
       <c r="B150" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C150" s="3">
         <v>43922</v>
       </c>
       <c r="D150" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -62726,13 +62721,13 @@
         <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C151" s="3">
         <v>43922</v>
       </c>
       <c r="D151" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -62740,13 +62735,13 @@
         <v>14</v>
       </c>
       <c r="B152" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C152" s="3">
         <v>43922</v>
       </c>
       <c r="D152" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -62754,13 +62749,13 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C153" s="3">
         <v>43922</v>
       </c>
       <c r="D153" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -62768,13 +62763,13 @@
         <v>18</v>
       </c>
       <c r="B154" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C154" s="3">
         <v>43922</v>
       </c>
       <c r="D154" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -62782,13 +62777,13 @@
         <v>16</v>
       </c>
       <c r="B155" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C155" s="3">
         <v>43923</v>
       </c>
       <c r="D155" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -62796,13 +62791,13 @@
         <v>13</v>
       </c>
       <c r="B156" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C156" s="3">
         <v>43923</v>
       </c>
       <c r="D156" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -62810,13 +62805,13 @@
         <v>12</v>
       </c>
       <c r="B157" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C157" s="3">
         <v>43923</v>
       </c>
       <c r="D157" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -62824,13 +62819,13 @@
         <v>14</v>
       </c>
       <c r="B158" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C158" s="3">
         <v>43923</v>
       </c>
       <c r="D158" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -62838,13 +62833,13 @@
         <v>17</v>
       </c>
       <c r="B159" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C159" s="3">
         <v>43923</v>
       </c>
       <c r="D159" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -62852,13 +62847,13 @@
         <v>18</v>
       </c>
       <c r="B160" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C160" s="3">
         <v>43923</v>
       </c>
       <c r="D160" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -62866,13 +62861,13 @@
         <v>16</v>
       </c>
       <c r="B161" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C161" s="3">
         <v>43924</v>
       </c>
       <c r="D161" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -62880,13 +62875,13 @@
         <v>16</v>
       </c>
       <c r="B162" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C162" s="3">
         <v>43924</v>
       </c>
       <c r="D162" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -62894,13 +62889,13 @@
         <v>13</v>
       </c>
       <c r="B163" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C163" s="3">
         <v>43924</v>
       </c>
       <c r="D163" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -62908,13 +62903,13 @@
         <v>12</v>
       </c>
       <c r="B164" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C164" s="3">
         <v>43924</v>
       </c>
       <c r="D164" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -62922,13 +62917,13 @@
         <v>14</v>
       </c>
       <c r="B165" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C165" s="3">
         <v>43924</v>
       </c>
       <c r="D165" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -62936,13 +62931,13 @@
         <v>17</v>
       </c>
       <c r="B166" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C166" s="3">
         <v>43924</v>
       </c>
       <c r="D166" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -62950,13 +62945,13 @@
         <v>18</v>
       </c>
       <c r="B167" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C167" s="3">
         <v>43924</v>
       </c>
       <c r="D167" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -62981,13 +62976,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>